<commit_message>
Vocab List 5 added
vocab list 5 added with answers
</commit_message>
<xml_diff>
--- a/WordsListUtil.xlsx
+++ b/WordsListUtil.xlsx
@@ -16,72 +16,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Gaiety</t>
-  </si>
-  <si>
-    <t>Jest</t>
-  </si>
-  <si>
-    <t>Jocular</t>
-  </si>
-  <si>
-    <t>Jocund</t>
-  </si>
-  <si>
-    <t>Jollity</t>
-  </si>
-  <si>
-    <t>Jovial</t>
-  </si>
-  <si>
-    <t>Jubilant</t>
-  </si>
-  <si>
-    <t>Rapturous</t>
-  </si>
-  <si>
-    <t>Regale</t>
-  </si>
-  <si>
-    <t>Sanguine</t>
-  </si>
-  <si>
-    <t>Uproaracious</t>
-  </si>
-  <si>
-    <t>Waggish</t>
-  </si>
-  <si>
-    <t>Cardinal</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Foremost</t>
-  </si>
-  <si>
-    <t>Imperative</t>
-  </si>
-  <si>
-    <t>Indispensible</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
-    <t>Momentuous</t>
-  </si>
-  <si>
-    <t>Paramount</t>
-  </si>
-  <si>
-    <t>Pivotal</t>
-  </si>
-  <si>
-    <t>Salient</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Plethora</t>
+  </si>
+  <si>
+    <t>Profuse</t>
+  </si>
+  <si>
+    <t>Prolific</t>
+  </si>
+  <si>
+    <t>Rife</t>
+  </si>
+  <si>
+    <t>Spate</t>
+  </si>
+  <si>
+    <t>Steeped</t>
+  </si>
+  <si>
+    <t>Surfeit</t>
+  </si>
+  <si>
+    <t>Surge</t>
+  </si>
+  <si>
+    <t>Teeming</t>
+  </si>
+  <si>
+    <t>Volley</t>
+  </si>
+  <si>
+    <t>Exiguous</t>
+  </si>
+  <si>
+    <t>Marginal</t>
+  </si>
+  <si>
+    <t>Meagre</t>
+  </si>
+  <si>
+    <t>Negligible</t>
+  </si>
+  <si>
+    <t>Paltry</t>
+  </si>
+  <si>
+    <t>Scanty</t>
+  </si>
+  <si>
+    <t>Skimpy</t>
+  </si>
+  <si>
+    <t>Spare</t>
+  </si>
+  <si>
+    <t>Sparse</t>
   </si>
 </sst>
 </file>
@@ -416,7 +407,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C1:C10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -428,288 +419,279 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="str">
         <f>CONCATENATE("public static final String ",UPPER(A1)," = ",""""&amp;A1&amp;"""",";")</f>
-        <v>public static final String CARDINAL = "Cardinal";</v>
+        <v>public static final String EXIGUOUS = "Exiguous";</v>
       </c>
       <c r="C1" t="str">
         <f>CONCATENATE(UPPER(A1)&amp;",")</f>
-        <v>CARDINAL,</v>
+        <v>EXIGUOUS,</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B22" si="0">CONCATENATE("public static final String ",UPPER(A2)," = ",""""&amp;A2&amp;"""",";")</f>
-        <v>public static final String CORE = "Core";</v>
+        <v>public static final String MARGINAL = "Marginal";</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C22" si="1">CONCATENATE(UPPER(A2)&amp;",")</f>
-        <v>CORE,</v>
+        <v>MARGINAL,</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String FOREMOST = "Foremost";</v>
+        <v>public static final String MEAGRE = "Meagre";</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="1"/>
-        <v>FOREMOST,</v>
+        <v>MEAGRE,</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String IMPERATIVE = "Imperative";</v>
+        <v>public static final String NEGLIGIBLE = "Negligible";</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
-        <v>IMPERATIVE,</v>
+        <v>NEGLIGIBLE,</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String INDISPENSIBLE = "Indispensible";</v>
+        <v>public static final String PALTRY = "Paltry";</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
-        <v>INDISPENSIBLE,</v>
+        <v>PALTRY,</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String MANDATORY = "Mandatory";</v>
+        <v>public static final String SCANTY = "Scanty";</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
-        <v>MANDATORY,</v>
+        <v>SCANTY,</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String MOMENTUOUS = "Momentuous";</v>
+        <v>public static final String SKIMPY = "Skimpy";</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>MOMENTUOUS,</v>
+        <v>SKIMPY,</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String PARAMOUNT = "Paramount";</v>
+        <v>public static final String SPARE = "Spare";</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>PARAMOUNT,</v>
+        <v>SPARE,</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String PIVOTAL = "Pivotal";</v>
+        <v>public static final String SPARSE = "Sparse";</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>PIVOTAL,</v>
+        <v>SPARSE,</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String SALIENT = "Salient";</v>
+        <v>public static final String PLETHORA = "Plethora";</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>SALIENT,</v>
+        <v>PLETHORA,</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String GAIETY = "Gaiety";</v>
+        <v>public static final String PROFUSE = "Profuse";</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>GAIETY,</v>
+        <v>PROFUSE,</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JEST = "Jest";</v>
+        <v>public static final String PROLIFIC = "Prolific";</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>JEST,</v>
+        <v>PROLIFIC,</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JOCULAR = "Jocular";</v>
+        <v>public static final String RIFE = "Rife";</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>JOCULAR,</v>
+        <v>RIFE,</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JOCUND = "Jocund";</v>
+        <v>public static final String SPATE = "Spate";</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>JOCUND,</v>
+        <v>SPATE,</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JOLLITY = "Jollity";</v>
+        <v>public static final String STEEPED = "Steeped";</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>JOLLITY,</v>
+        <v>STEEPED,</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JOVIAL = "Jovial";</v>
+        <v>public static final String SURFEIT = "Surfeit";</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
-        <v>JOVIAL,</v>
+        <v>SURFEIT,</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String JUBILANT = "Jubilant";</v>
+        <v>public static final String SURGE = "Surge";</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
-        <v>JUBILANT,</v>
+        <v>SURGE,</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String RAPTUROUS = "Rapturous";</v>
+        <v>public static final String TEEMING = "Teeming";</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
-        <v>RAPTUROUS,</v>
+        <v>TEEMING,</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String REGALE = "Regale";</v>
+        <v>public static final String VOLLEY = "Volley";</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
-        <v>REGALE,</v>
+        <v>VOLLEY,</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String SANGUINE = "Sanguine";</v>
+        <v>public static final String  = "";</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
-        <v>SANGUINE,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String UPROARACIOUS = "Uproaracious";</v>
+        <v>public static final String  = "";</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
-        <v>UPROARACIOUS,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>public static final String WAGGISH = "Waggish";</v>
+        <v>public static final String  = "";</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
-        <v>WAGGISH,</v>
+        <v>,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>